<commit_message>
all spj done minus pdf
</commit_message>
<xml_diff>
--- a/public/DataSPJ/spj honor dosen.xlsx
+++ b/public/DataSPJ/spj honor dosen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F70006-3195-48A4-B7EA-237381B941F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427C7507-83C3-47CB-AA20-65A6248DAE32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="1170" windowWidth="11010" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="honor" sheetId="1" r:id="rId1"/>
@@ -114,13 +114,13 @@
     <t>d</t>
   </si>
   <si>
-    <t>qq</t>
+    <t>a</t>
   </si>
   <si>
-    <t>ww</t>
+    <t>b</t>
   </si>
   <si>
-    <t>ee</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -538,10 +538,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -675,11 +675,11 @@
         <v>25</v>
       </c>
       <c r="C3" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="10">
         <f>IF(C3=1, 100, IF(C3=2, 200, IF(C3=3, 300, "400")))</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E3" s="11">
         <v>3</v>
@@ -692,15 +692,15 @@
       </c>
       <c r="H3" s="10">
         <f>D3*G3</f>
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I3" s="10">
         <f>0.25*H3</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J3" s="10">
         <f>H3-I3</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="K3" s="12">
         <v>11111111</v>
@@ -734,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D5" si="0">IF(C4=1, 100, IF(C4=2, 200, IF(C4=3, 300, "400")))</f>
+        <f t="shared" ref="D4" si="0">IF(C4=1, 100, IF(C4=2, 200, IF(C4=3, 300, "400")))</f>
         <v>200</v>
       </c>
       <c r="E4" s="11">
@@ -751,11 +751,11 @@
         <v>400</v>
       </c>
       <c r="I4" s="10">
-        <f t="shared" ref="I4:I5" si="2">0.25*H4</f>
+        <f t="shared" ref="I4" si="2">0.25*H4</f>
         <v>100</v>
       </c>
       <c r="J4" s="10">
-        <f t="shared" ref="J4:J5" si="3">H4-I4</f>
+        <f t="shared" ref="J4" si="3">H4-I4</f>
         <v>300</v>
       </c>
       <c r="K4" s="12">
@@ -787,11 +787,11 @@
         <v>27</v>
       </c>
       <c r="C5" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="10">
-        <f t="shared" si="0"/>
-        <v>300</v>
+        <f>IF(C5=1, 100, IF(C5=2, 200, IF(C5=3, 300, "400")))</f>
+        <v>200</v>
       </c>
       <c r="E5" s="11">
         <v>3</v>
@@ -804,15 +804,15 @@
       </c>
       <c r="H5" s="10">
         <f>D5*G5</f>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="I5" s="10">
-        <f t="shared" si="2"/>
-        <v>150</v>
+        <f>0.25*H5</f>
+        <v>100</v>
       </c>
       <c r="J5" s="10">
-        <f t="shared" si="3"/>
-        <v>450</v>
+        <f>H5-I5</f>
+        <v>300</v>
       </c>
       <c r="K5" s="12">
         <v>11111111</v>
@@ -865,16 +865,16 @@
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="13"/>
       <c r="D7" s="2"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="14"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="13"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -893,16 +893,16 @@
     </row>
     <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="13"/>
       <c r="D8" s="2"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="13"/>
       <c r="H8" s="14"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="15"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -921,16 +921,16 @@
     </row>
     <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="13"/>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -28303,34 +28303,6 @@
       <c r="Y986" s="1"/>
       <c r="Z986" s="1"/>
     </row>
-    <row r="987" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="C987" s="1"/>
-      <c r="D987" s="2"/>
-      <c r="E987" s="1"/>
-      <c r="F987" s="1"/>
-      <c r="G987" s="1"/>
-      <c r="H987" s="1"/>
-      <c r="I987" s="1"/>
-      <c r="J987" s="1"/>
-      <c r="K987" s="1"/>
-      <c r="L987" s="1"/>
-      <c r="M987" s="1"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="1"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-      <c r="T987" s="1"/>
-      <c r="U987" s="1"/>
-      <c r="V987" s="1"/>
-      <c r="W987" s="1"/>
-      <c r="X987" s="1"/>
-      <c r="Y987" s="1"/>
-      <c r="Z987" s="1"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:J3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>